<commit_message>
changes made to stories 1,2
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint2BacklogV2.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint2BacklogV2.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22325"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\The king\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afzalmiah\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8F8DE6D-6D68-48A1-8133-B66BC5B6C9D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Agile Sprint Backlog" sheetId="5" r:id="rId1"/>
@@ -21,7 +20,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$W$27</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Agile Sprint Backlog - BLANK'!$B$2:$V$28</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="67">
   <si>
     <t>User Story #1</t>
   </si>
@@ -206,9 +205,6 @@
     <t>To Do</t>
   </si>
   <si>
-    <t>Development</t>
-  </si>
-  <si>
     <t>2. validate the two search boxes to disallow a search when both search boxes are not null</t>
   </si>
   <si>
@@ -245,7 +241,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -427,7 +423,7 @@
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -489,6 +485,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -539,16 +536,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>41</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>15.5</c:v>
+                  <c:v>18.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -1292,7 +1289,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
@@ -1301,7 +1298,7 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.75" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1418,7 +1415,9 @@
       </c>
       <c r="D3" s="8"/>
       <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="F3" s="8" t="s">
+        <v>66</v>
+      </c>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -1453,7 +1452,7 @@
       </c>
       <c r="E4" s="9"/>
       <c r="F4" s="9" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G4" s="9">
         <v>4</v>
@@ -1465,7 +1464,7 @@
         <v>2</v>
       </c>
       <c r="J4" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="9">
         <v>0</v>
@@ -1503,7 +1502,7 @@
       </c>
       <c r="E5" s="9"/>
       <c r="F5" s="9" t="s">
-        <v>56</v>
+        <v>66</v>
       </c>
       <c r="G5" s="9">
         <v>11</v>
@@ -1515,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="9">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="K5" s="9">
         <v>0</v>
@@ -1553,7 +1552,7 @@
       </c>
       <c r="E6" s="9"/>
       <c r="F6" s="9" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G6" s="9">
         <v>5</v>
@@ -1565,7 +1564,7 @@
         <v>0</v>
       </c>
       <c r="J6" s="9">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K6" s="9">
         <v>0</v>
@@ -1687,19 +1686,19 @@
         <v>50</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G9" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H9" s="9">
         <v>0</v>
       </c>
       <c r="I9" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K9" s="9">
         <v>0</v>
@@ -1737,10 +1736,10 @@
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="G10" s="9">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H10" s="9">
         <v>0</v>
@@ -1749,7 +1748,7 @@
         <v>0</v>
       </c>
       <c r="J10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K10" s="9">
         <v>0</v>
@@ -1787,10 +1786,10 @@
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="G11" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H11" s="9">
         <v>0</v>
@@ -1799,7 +1798,7 @@
         <v>0</v>
       </c>
       <c r="J11" s="9">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K11" s="9">
         <v>0</v>
@@ -1883,7 +1882,7 @@
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -1911,7 +1910,7 @@
     </row>
     <row r="14" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9" t="s">
@@ -1919,7 +1918,7 @@
       </c>
       <c r="E14" s="9"/>
       <c r="F14" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" s="9">
         <v>2</v>
@@ -1961,7 +1960,7 @@
     </row>
     <row r="15" spans="2:29" ht="25.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9" t="s">
@@ -1969,7 +1968,7 @@
       </c>
       <c r="E15" s="9"/>
       <c r="F15" s="9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G15" s="9">
         <v>1</v>
@@ -2065,7 +2064,7 @@
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
       <c r="F17" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -2101,7 +2100,7 @@
       </c>
       <c r="E18" s="9"/>
       <c r="F18" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G18" s="9">
         <v>3</v>
@@ -2151,7 +2150,7 @@
       </c>
       <c r="E19" s="9"/>
       <c r="F19" s="9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G19" s="9">
         <v>1</v>
@@ -2247,7 +2246,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -2285,7 +2284,7 @@
         <v>51</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G22" s="9">
         <v>1</v>
@@ -2335,7 +2334,7 @@
       </c>
       <c r="E23" s="9"/>
       <c r="F23" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G23" s="9">
         <v>1</v>
@@ -2477,7 +2476,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
       <c r="F26" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G26" s="8"/>
       <c r="H26" s="8"/>
@@ -2515,7 +2514,7 @@
         <v>52</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G27" s="9">
         <v>1</v>
@@ -2565,7 +2564,7 @@
       </c>
       <c r="E28" s="9"/>
       <c r="F28" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G28" s="9">
         <v>1</v>
@@ -2707,7 +2706,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="8"/>
       <c r="F31" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G31" s="8"/>
       <c r="H31" s="8"/>
@@ -2743,7 +2742,7 @@
       </c>
       <c r="E32" s="9"/>
       <c r="F32" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G32" s="9">
         <v>1</v>
@@ -2793,7 +2792,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="8"/>
       <c r="F33" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G33" s="8"/>
       <c r="H33" s="8"/>
@@ -2829,7 +2828,7 @@
       </c>
       <c r="E34" s="9"/>
       <c r="F34" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G34" s="9">
         <v>2</v>
@@ -3017,7 +3016,7 @@
       <c r="D38" s="8"/>
       <c r="E38" s="8"/>
       <c r="F38" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G38" s="8"/>
       <c r="H38" s="8"/>
@@ -3045,7 +3044,7 @@
     </row>
     <row r="39" spans="2:29" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C39" s="9"/>
       <c r="D39" s="9" t="s">
@@ -3053,7 +3052,7 @@
       </c>
       <c r="E39" s="9"/>
       <c r="F39" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G39" s="9">
         <v>1</v>
@@ -3095,7 +3094,7 @@
     </row>
     <row r="40" spans="2:29" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C40" s="9"/>
       <c r="D40" s="9" t="s">
@@ -3103,7 +3102,7 @@
       </c>
       <c r="E40" s="9"/>
       <c r="F40" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G40" s="9">
         <v>3</v>
@@ -3145,7 +3144,7 @@
     </row>
     <row r="41" spans="2:29" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C41" s="9"/>
       <c r="D41" s="9" t="s">
@@ -3153,7 +3152,7 @@
       </c>
       <c r="E41" s="9"/>
       <c r="F41" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G41" s="9">
         <v>1</v>
@@ -3195,7 +3194,7 @@
     </row>
     <row r="42" spans="2:29" ht="40.5" x14ac:dyDescent="0.25">
       <c r="B42" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C42" s="9"/>
       <c r="D42" s="9" t="s">
@@ -3203,7 +3202,7 @@
       </c>
       <c r="E42" s="9"/>
       <c r="F42" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G42" s="9">
         <v>2</v>
@@ -3479,7 +3478,7 @@
       <c r="F48" s="5"/>
       <c r="G48" s="5">
         <f>SUM(G3:G47)</f>
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="H48" s="5">
         <f>SUM(H4:H47)</f>
@@ -3487,11 +3486,11 @@
       </c>
       <c r="I48" s="5">
         <f>SUM(I3:I47)</f>
-        <v>15.5</v>
+        <v>18.5</v>
       </c>
       <c r="J48" s="5">
         <f>SUM(J3:J47)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="K48" s="5">
         <f>SUM(K3:K47)</f>
@@ -6047,7 +6046,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3" tint="0.39997558519241921"/>
     <pageSetUpPr fitToPage="1"/>
@@ -9752,7 +9751,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="1"/>
   </sheetPr>

</xml_diff>